<commit_message>
fixed a bug in reading excel files. trimming oputer shouldnt be called for excel files
</commit_message>
<xml_diff>
--- a/development/TestExcel1.xlsx
+++ b/development/TestExcel1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,25 +23,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x2</t>
+  </si>
+  <si>
     <t xml:space="preserve">d</t>
   </si>
   <si>
     <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
   </si>
   <si>
     <t xml:space="preserve">f</t>
@@ -251,69 +251,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B10:D14"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="B2:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -324,18 +261,18 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1.1</v>
@@ -346,7 +283,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2</v>
@@ -357,7 +294,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -368,7 +305,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
@@ -379,10 +316,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H12" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>7</v>
@@ -390,7 +327,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>1.1</v>
@@ -401,7 +338,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="1" t="n">
         <v>2</v>
@@ -412,7 +349,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H15" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="1" t="n">
         <v>2</v>
@@ -423,7 +360,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H16" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1" t="n">
         <v>1</v>
@@ -441,4 +378,67 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B10:D14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added multi table support
</commit_message>
<xml_diff>
--- a/development/TestExcel1.xlsx
+++ b/development/TestExcel1.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -32,19 +31,40 @@
     <t xml:space="preserve">c</t>
   </si>
   <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
     <t xml:space="preserve">x1</t>
   </si>
   <si>
     <t xml:space="preserve">x2</t>
   </si>
   <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
+    <t xml:space="preserve">k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j</t>
   </si>
 </sst>
 </file>
@@ -119,12 +139,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,8 +277,8 @@
   </sheetPr>
   <dimension ref="B2:J16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -269,10 +293,19 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1.1</v>
@@ -280,21 +313,39 @@
       <c r="D3" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="G3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>2</v>
@@ -305,7 +356,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
@@ -314,60 +365,130 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -378,67 +499,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B10:D14"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>